<commit_message>
updated for 40 epochs
</commit_message>
<xml_diff>
--- a/combined.xlsx
+++ b/combined.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pulki\OneDrive\Desktop\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1F0D41-7F5D-4D8B-B3F4-0D589E6863DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB32FBD8-E70F-4E97-AD7E-2FF9725EA5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1D7F0558-AE29-4457-9EF5-40EDE7F373B8}"/>
   </bookViews>
   <sheets>
-    <sheet name="combine" sheetId="2" r:id="rId1"/>
+    <sheet name="combine (2)" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="14">
   <si>
     <t>epoch</t>
   </si>
@@ -72,13 +72,7 @@
     <t>false positive rate</t>
   </si>
   <si>
-    <t>error</t>
-  </si>
-  <si>
     <t>tanh</t>
-  </si>
-  <si>
-    <t>relu</t>
   </si>
   <si>
     <t>sigm</t>
@@ -452,11 +446,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470AB296-600B-4B86-AFA9-59F6B1757E59}">
-  <dimension ref="A1:M51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE130999-3F1F-4A52-847D-E82A789A04F2}">
+  <dimension ref="A1:M67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,16 +502,14 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -552,7 +544,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>150</v>
@@ -587,7 +579,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>200</v>
@@ -622,7 +614,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>250</v>
@@ -657,7 +649,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>300</v>
@@ -692,7 +684,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>350</v>
@@ -727,7 +719,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>400</v>
@@ -762,7 +754,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>500</v>
@@ -797,7 +789,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>100</v>
@@ -828,9 +820,6 @@
       </c>
       <c r="L10">
         <v>0.394175078603342</v>
-      </c>
-      <c r="M10">
-        <v>0.24229843062359799</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -838,7 +827,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>150</v>
@@ -876,7 +865,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>200</v>
@@ -907,9 +896,6 @@
       </c>
       <c r="L12">
         <v>0.36505047162005599</v>
-      </c>
-      <c r="M12">
-        <v>0.210412687868471</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -917,7 +903,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>250</v>
@@ -948,9 +934,6 @@
       </c>
       <c r="L13">
         <v>0.349826245242429</v>
-      </c>
-      <c r="M13">
-        <v>0.20385286058291099</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -958,7 +941,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>300</v>
@@ -996,7 +979,7 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>350</v>
@@ -1027,9 +1010,6 @@
       </c>
       <c r="L15">
         <v>0.34403441999007101</v>
-      </c>
-      <c r="M15">
-        <v>0.192393921780287</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1037,7 +1017,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>400</v>
@@ -1069,16 +1049,13 @@
       <c r="L16">
         <v>0.33791163329472101</v>
       </c>
-      <c r="M16">
-        <v>0.18558498712945201</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17">
         <v>500</v>
@@ -1111,12 +1088,12 @@
         <v>0.30746318053946697</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18">
         <v>100</v>
@@ -1149,12 +1126,12 @@
         <v>0.37597219923878866</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19">
         <v>150</v>
@@ -1187,12 +1164,12 @@
         <v>0.34370345854707929</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20">
         <v>200</v>
@@ -1225,12 +1202,12 @@
         <v>0.35694191626675498</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21">
         <v>250</v>
@@ -1263,12 +1240,12 @@
         <v>0.31507529372828069</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22">
         <v>300</v>
@@ -1301,12 +1278,12 @@
         <v>0.33410557670031438</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23">
         <v>350</v>
@@ -1339,12 +1316,12 @@
         <v>0.29885818302167799</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24">
         <v>400</v>
@@ -1377,12 +1354,12 @@
         <v>0.30200231673010092</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25">
         <v>450</v>
@@ -1415,12 +1392,12 @@
         <v>0.2808207843786199</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26">
         <v>500</v>
@@ -1453,12 +1430,12 @@
         <v>0.27469799768326986</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C27">
         <v>100</v>
@@ -1490,16 +1467,13 @@
       <c r="L27">
         <v>0.35098461029290084</v>
       </c>
-      <c r="M27">
-        <v>0.21938055301835091</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C28">
         <v>150</v>
@@ -1531,16 +1505,13 @@
       <c r="L28">
         <v>0.35181201390038064</v>
       </c>
-      <c r="M28">
-        <v>0.21738769409615544</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C29">
         <v>200</v>
@@ -1573,12 +1544,12 @@
         <v>0.36124441502564952</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C30">
         <v>250</v>
@@ -1610,16 +1581,13 @@
       <c r="L30">
         <v>0.32864471289094821</v>
       </c>
-      <c r="M30">
-        <v>0.19048409864651664</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C31">
         <v>300</v>
@@ -1651,16 +1619,13 @@
       <c r="L31">
         <v>0.32864471289094821</v>
       </c>
-      <c r="M31">
-        <v>0.19048409864651664</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C32">
         <v>350</v>
@@ -1693,12 +1658,12 @@
         <v>0.32748634784047659</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C33">
         <v>400</v>
@@ -1730,16 +1695,13 @@
       <c r="L33">
         <v>0.31788846599371168</v>
       </c>
-      <c r="M33">
-        <v>0.1781948019596446</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C34">
         <v>450</v>
@@ -1772,12 +1734,12 @@
         <v>0.32715538639748465</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C35">
         <v>500</v>
@@ -1810,12 +1772,12 @@
         <v>0.31540625517127252</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C36">
         <v>100</v>
@@ -1848,12 +1810,12 @@
         <v>0.35992056925368199</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C37">
         <v>150</v>
@@ -1886,12 +1848,12 @@
         <v>0.33360913453582652</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C38">
         <v>200</v>
@@ -1924,12 +1886,12 @@
         <v>0.32649346351150088</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C39">
         <v>250</v>
@@ -1962,12 +1924,12 @@
         <v>0.301836836008605</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>30</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C40">
         <v>300</v>
@@ -2000,12 +1962,12 @@
         <v>0.30150587456561306</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>30</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C41">
         <v>350</v>
@@ -2038,12 +2000,12 @@
         <v>0.30216779745159694</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>30</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C42">
         <v>400</v>
@@ -2076,12 +2038,12 @@
         <v>0.29621049147774281</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>30</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C43">
         <v>500</v>
@@ -2114,12 +2076,12 @@
         <v>0.2646036736720172</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C44">
         <v>100</v>
@@ -2152,12 +2114,12 @@
         <v>0.39268575210987922</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>30</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C45">
         <v>150</v>
@@ -2190,12 +2152,12 @@
         <v>0.36356114512659277</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>30</v>
       </c>
       <c r="B46" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C46">
         <v>200</v>
@@ -2228,12 +2190,12 @@
         <v>0.35992056925368199</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>30</v>
       </c>
       <c r="B47" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C47">
         <v>250</v>
@@ -2266,12 +2228,12 @@
         <v>0.32748634784047659</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>30</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C48">
         <v>300</v>
@@ -2309,7 +2271,7 @@
         <v>30</v>
       </c>
       <c r="B49" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C49">
         <v>350</v>
@@ -2347,7 +2309,7 @@
         <v>30</v>
       </c>
       <c r="B50" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C50">
         <v>400</v>
@@ -2385,7 +2347,7 @@
         <v>30</v>
       </c>
       <c r="B51" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C51">
         <v>500</v>
@@ -2416,6 +2378,614 @@
       </c>
       <c r="L51">
         <v>0.32516961773953335</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>40</v>
+      </c>
+      <c r="B52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52">
+        <v>100</v>
+      </c>
+      <c r="D52">
+        <v>2.5353901386260902</v>
+      </c>
+      <c r="E52">
+        <v>1.7272562980651855</v>
+      </c>
+      <c r="F52">
+        <v>0.7007646985082111</v>
+      </c>
+      <c r="G52">
+        <v>0.93166666666666664</v>
+      </c>
+      <c r="H52">
+        <v>0.79988552622164988</v>
+      </c>
+      <c r="I52">
+        <v>0.76774889977580341</v>
+      </c>
+      <c r="J52">
+        <v>0.93166666666666664</v>
+      </c>
+      <c r="K52">
+        <v>0.60499751778917754</v>
+      </c>
+      <c r="L52">
+        <v>0.39500248221082246</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>40</v>
+      </c>
+      <c r="B53" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53">
+        <v>150</v>
+      </c>
+      <c r="D53">
+        <v>3.10221219062805</v>
+      </c>
+      <c r="E53">
+        <v>2.1093511581420898</v>
+      </c>
+      <c r="F53">
+        <v>0.74321340433822569</v>
+      </c>
+      <c r="G53">
+        <v>0.95366666666666666</v>
+      </c>
+      <c r="H53">
+        <v>0.83538944448499886</v>
+      </c>
+      <c r="I53">
+        <v>0.81275429710205094</v>
+      </c>
+      <c r="J53">
+        <v>0.95366666666666666</v>
+      </c>
+      <c r="K53">
+        <v>0.67284461360251535</v>
+      </c>
+      <c r="L53">
+        <v>0.32715538639748465</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>40</v>
+      </c>
+      <c r="B54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54">
+        <v>200</v>
+      </c>
+      <c r="D54">
+        <v>2.9938716888427699</v>
+      </c>
+      <c r="E54">
+        <v>1.9867029190063477</v>
+      </c>
+      <c r="F54">
+        <v>0.74515839425420038</v>
+      </c>
+      <c r="G54">
+        <v>0.96833333333333338</v>
+      </c>
+      <c r="H54">
+        <v>0.84221207508878748</v>
+      </c>
+      <c r="I54">
+        <v>0.81923108859918625</v>
+      </c>
+      <c r="J54">
+        <v>0.96833333333333338</v>
+      </c>
+      <c r="K54">
+        <v>0.67118980638755588</v>
+      </c>
+      <c r="L54">
+        <v>0.32881019361244412</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>40</v>
+      </c>
+      <c r="B55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55">
+        <v>250</v>
+      </c>
+      <c r="D55">
+        <v>3.2353205680847101</v>
+      </c>
+      <c r="E55">
+        <v>2.1876082420349121</v>
+      </c>
+      <c r="F55">
+        <v>0.75605626465225317</v>
+      </c>
+      <c r="G55">
+        <v>0.96750000000000003</v>
+      </c>
+      <c r="H55">
+        <v>0.8488083053077935</v>
+      </c>
+      <c r="I55">
+        <v>0.82828198953749066</v>
+      </c>
+      <c r="J55">
+        <v>0.96750000000000003</v>
+      </c>
+      <c r="K55">
+        <v>0.69005460863809365</v>
+      </c>
+      <c r="L55">
+        <v>0.30994539136190635</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>40</v>
+      </c>
+      <c r="B56" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56">
+        <v>300</v>
+      </c>
+      <c r="D56">
+        <v>3.52563023567199</v>
+      </c>
+      <c r="E56">
+        <v>2.2905526161193848</v>
+      </c>
+      <c r="F56">
+        <v>0.75973434040890742</v>
+      </c>
+      <c r="G56">
+        <v>0.97233333333333338</v>
+      </c>
+      <c r="H56">
+        <v>0.8529863294100446</v>
+      </c>
+      <c r="I56">
+        <v>0.83301502947770489</v>
+      </c>
+      <c r="J56">
+        <v>0.97233333333333338</v>
+      </c>
+      <c r="K56">
+        <v>0.69468806883998013</v>
+      </c>
+      <c r="L56">
+        <v>0.30531193116001987</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>40</v>
+      </c>
+      <c r="B57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57">
+        <v>350</v>
+      </c>
+      <c r="D57">
+        <v>3.8781893253326398</v>
+      </c>
+      <c r="E57">
+        <v>2.3223521709442139</v>
+      </c>
+      <c r="F57">
+        <v>0.75481203978814104</v>
+      </c>
+      <c r="G57">
+        <v>0.97383333333333333</v>
+      </c>
+      <c r="H57">
+        <v>0.85044756567935376</v>
+      </c>
+      <c r="I57">
+        <v>0.82936145478701317</v>
+      </c>
+      <c r="J57">
+        <v>0.97383333333333333</v>
+      </c>
+      <c r="K57">
+        <v>0.68591759060069502</v>
+      </c>
+      <c r="L57">
+        <v>0.31408240939930498</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>40</v>
+      </c>
+      <c r="B58" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58">
+        <v>400</v>
+      </c>
+      <c r="D58">
+        <v>4.0881648063659597</v>
+      </c>
+      <c r="E58">
+        <v>2.0987629890441895</v>
+      </c>
+      <c r="F58">
+        <v>0.77139847247827231</v>
+      </c>
+      <c r="G58">
+        <v>0.97633333333333339</v>
+      </c>
+      <c r="H58">
+        <v>0.86185081653670725</v>
+      </c>
+      <c r="I58">
+        <v>0.84405878933820477</v>
+      </c>
+      <c r="J58">
+        <v>0.97633333333333339</v>
+      </c>
+      <c r="K58">
+        <v>0.71272546748303822</v>
+      </c>
+      <c r="L58">
+        <v>0.28727453251696178</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>40</v>
+      </c>
+      <c r="B59" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59">
+        <v>500</v>
+      </c>
+      <c r="D59">
+        <v>4.6244003772735596</v>
+      </c>
+      <c r="E59">
+        <v>2.6036369800567627</v>
+      </c>
+      <c r="F59">
+        <v>0.78579059829059827</v>
+      </c>
+      <c r="G59">
+        <v>0.98066666666666669</v>
+      </c>
+      <c r="H59">
+        <v>0.87247924080664296</v>
+      </c>
+      <c r="I59">
+        <v>0.85717844390932496</v>
+      </c>
+      <c r="J59">
+        <v>0.98066666666666669</v>
+      </c>
+      <c r="K59">
+        <v>0.73456892272050311</v>
+      </c>
+      <c r="L59">
+        <v>0.26543107727949689</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>40</v>
+      </c>
+      <c r="B60" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60">
+        <v>100</v>
+      </c>
+      <c r="D60">
+        <v>7.3112034797668404</v>
+      </c>
+      <c r="E60">
+        <v>1.9119291305541992</v>
+      </c>
+      <c r="F60">
+        <v>0.69467752035065744</v>
+      </c>
+      <c r="G60">
+        <v>0.92449999999999999</v>
+      </c>
+      <c r="H60">
+        <v>0.7932785126921702</v>
+      </c>
+      <c r="I60">
+        <v>0.75994353566387118</v>
+      </c>
+      <c r="J60">
+        <v>0.92449999999999999</v>
+      </c>
+      <c r="K60">
+        <v>0.59655800099288436</v>
+      </c>
+      <c r="L60">
+        <v>0.40344199900711564</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>40</v>
+      </c>
+      <c r="B61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61">
+        <v>150</v>
+      </c>
+      <c r="D61">
+        <v>2.7228543758392298</v>
+      </c>
+      <c r="E61">
+        <v>2.0995926856994629</v>
+      </c>
+      <c r="F61">
+        <v>0.72357096981374436</v>
+      </c>
+      <c r="G61">
+        <v>0.9388333333333333</v>
+      </c>
+      <c r="H61">
+        <v>0.8172651432716721</v>
+      </c>
+      <c r="I61">
+        <v>0.79083284895790085</v>
+      </c>
+      <c r="J61">
+        <v>0.9388333333333333</v>
+      </c>
+      <c r="K61">
+        <v>0.64388548734072482</v>
+      </c>
+      <c r="L61">
+        <v>0.35611451265927518</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>40</v>
+      </c>
+      <c r="B62" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62">
+        <v>200</v>
+      </c>
+      <c r="D62">
+        <v>3.0789587497711102</v>
+      </c>
+      <c r="E62">
+        <v>2.2872562408447266</v>
+      </c>
+      <c r="F62">
+        <v>0.72655754345895196</v>
+      </c>
+      <c r="G62">
+        <v>0.95433333333333337</v>
+      </c>
+      <c r="H62">
+        <v>0.82501260716086744</v>
+      </c>
+      <c r="I62">
+        <v>0.79830606991613384</v>
+      </c>
+      <c r="J62">
+        <v>0.95433333333333337</v>
+      </c>
+      <c r="K62">
+        <v>0.64338904517623696</v>
+      </c>
+      <c r="L62">
+        <v>0.35661095482376304</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>40</v>
+      </c>
+      <c r="B63" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63">
+        <v>250</v>
+      </c>
+      <c r="D63">
+        <v>3.2517404556274401</v>
+      </c>
+      <c r="E63">
+        <v>1.827782154083252</v>
+      </c>
+      <c r="F63">
+        <v>0.73116503620886797</v>
+      </c>
+      <c r="G63">
+        <v>0.95916666666666661</v>
+      </c>
+      <c r="H63">
+        <v>0.82978876793309775</v>
+      </c>
+      <c r="I63">
+        <v>0.80395250352902103</v>
+      </c>
+      <c r="J63">
+        <v>0.95916666666666661</v>
+      </c>
+      <c r="K63">
+        <v>0.64984279331457884</v>
+      </c>
+      <c r="L63">
+        <v>0.35015720668542116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>40</v>
+      </c>
+      <c r="B64" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64">
+        <v>300</v>
+      </c>
+      <c r="D64">
+        <v>3.6638770103454501</v>
+      </c>
+      <c r="E64">
+        <v>2.18377685546875</v>
+      </c>
+      <c r="F64">
+        <v>0.73123887051640801</v>
+      </c>
+      <c r="G64">
+        <v>0.95816666666666672</v>
+      </c>
+      <c r="H64">
+        <v>0.82946183811859764</v>
+      </c>
+      <c r="I64">
+        <v>0.80370339616374653</v>
+      </c>
+      <c r="J64">
+        <v>0.95816666666666672</v>
+      </c>
+      <c r="K64">
+        <v>0.65033923547906669</v>
+      </c>
+      <c r="L64">
+        <v>0.34966076452093331</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>40</v>
+      </c>
+      <c r="B65" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65">
+        <v>350</v>
+      </c>
+      <c r="D65">
+        <v>3.9214491844177202</v>
+      </c>
+      <c r="E65">
+        <v>1.9856235980987549</v>
+      </c>
+      <c r="F65">
+        <v>0.75116701244813278</v>
+      </c>
+      <c r="G65">
+        <v>0.96550000000000002</v>
+      </c>
+      <c r="H65">
+        <v>0.84495332555425895</v>
+      </c>
+      <c r="I65">
+        <v>0.82346591380885159</v>
+      </c>
+      <c r="J65">
+        <v>0.96550000000000002</v>
+      </c>
+      <c r="K65">
+        <v>0.68244249544928015</v>
+      </c>
+      <c r="L65">
+        <v>0.31755750455071985</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>40</v>
+      </c>
+      <c r="B66" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66">
+        <v>400</v>
+      </c>
+      <c r="D66">
+        <v>4.1701014041900599</v>
+      </c>
+      <c r="E66">
+        <v>2.6771097183227539</v>
+      </c>
+      <c r="F66">
+        <v>0.74990316333118145</v>
+      </c>
+      <c r="G66">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="H66">
+        <v>0.8451073117497272</v>
+      </c>
+      <c r="I66">
+        <v>0.8232168064435772</v>
+      </c>
+      <c r="J66">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="K66">
+        <v>0.67946384246235314</v>
+      </c>
+      <c r="L66">
+        <v>0.32053615753764686</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>40</v>
+      </c>
+      <c r="B67" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67">
+        <v>500</v>
+      </c>
+      <c r="D67">
+        <v>4.8614315986632999</v>
+      </c>
+      <c r="E67">
+        <v>3.2281332015991211</v>
+      </c>
+      <c r="F67">
+        <v>0.76675849403122132</v>
+      </c>
+      <c r="G67">
+        <v>0.97416666666666663</v>
+      </c>
+      <c r="H67">
+        <v>0.85810761212655073</v>
+      </c>
+      <c r="I67">
+        <v>0.83949182097484021</v>
+      </c>
+      <c r="J67">
+        <v>0.97416666666666663</v>
+      </c>
+      <c r="K67">
+        <v>0.70577527718020849</v>
+      </c>
+      <c r="L67">
+        <v>0.29422472281979151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>